<commit_message>
updated readme on fragility
</commit_message>
<xml_diff>
--- a/KCOR_Deviation_by_Age_and_Frailty.xlsx
+++ b/KCOR_Deviation_by_Age_and_Frailty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\KCOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6AF430EB-1423-4687-9D9B-9B8C06DDF018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CD7E2FA7-4879-4D87-9E15-6FCDAF4DCD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{B3B50EB5-49AA-4A9A-B525-3CEEA2714A21}"/>
   </bookViews>
@@ -55,7 +55,7 @@
     <t>Note that this table uses frailty which is constant for a cohort. It is NOT the ACM ratio of vaxxed/unvaxxed. You have to use the other spreadsheet, measure the ACM ratio and back it into find the correct frailty factor for the cohort you are observing.</t>
   </si>
   <si>
-    <t>KCOR deviation caused by frailty and age of the cohort</t>
+    <t>Given a frailty ratio and age, shows the KCOR distortion for that cohort</t>
   </si>
 </sst>
 </file>
@@ -921,7 +921,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>